<commit_message>
feat: update rules and enable live deployment
</commit_message>
<xml_diff>
--- a/src/brms_files/rules/waste/waste-rules-1.xlsx
+++ b/src/brms_files/rules/waste/waste-rules-1.xlsx
@@ -4,20 +4,19 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="clasification" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="clasification rule docs" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="UU4/F/nkt8vNXuJAp+8LKEo0Vj0r8rnJGpQu+F3GuDk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="w+etDmS2yssNwGQJa+1d+6CKJ8TufCHYjICz9NHpci8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>SimpleRules Integer clasification (String stateWaste, Integer weightInKg, Integer isotopesNumber)</t>
   </si>
@@ -37,7 +36,7 @@
     <t>solid</t>
   </si>
   <si>
-    <t>60 .. 120</t>
+    <t>0 .. 120</t>
   </si>
   <si>
     <t xml:space="preserve"> 1 .. 20</t>
@@ -67,7 +66,7 @@
     <t>gaseous</t>
   </si>
   <si>
-    <t>4 .. 8</t>
+    <t>0 .. 8</t>
   </si>
   <si>
     <t>8 .. 16</t>
@@ -86,22 +85,6 @@
   </si>
   <si>
     <t>121 .. 200</t>
-  </si>
-  <si>
-    <t>results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASD
-ALG
-BSD
-BLG
-CSD
-CLG
-DSD
-DLG
-ESD
-ELG
-</t>
   </si>
 </sst>
 </file>
@@ -137,7 +120,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,14 +151,8 @@
         <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7B7B7"/>
-        <bgColor rgb="FFB7B7B7"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="8">
     <border/>
     <border>
       <left style="thin">
@@ -251,53 +228,11 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -344,17 +279,6 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -364,10 +288,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3992,120 +3912,37 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:B15"/>
     <mergeCell ref="B16:B27"/>
     <mergeCell ref="B28:B39"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B40:B43"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B40:B43"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
     <mergeCell ref="E12:E15"/>
     <mergeCell ref="E16:E19"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E36:E37"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="2">
-      <c r="B2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3">
-      <c r="B3" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4">
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5">
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6">
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C16"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>